<commit_message>
SUBJECT: Added tool to generate yaml / JSON
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,37 +407,26 @@
         <v>resourceName</v>
       </c>
       <c r="B1" t="str">
-        <v>accountIds</v>
+        <v>accountId</v>
       </c>
       <c r="C1" t="str">
-        <v>regions</v>
+        <v>region</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>testResource</v>
-      </c>
-      <c r="B2" t="str">
-        <v>060087218145</v>
+        <v>shubhamTest</v>
+      </c>
+      <c r="B2">
+        <v>3438</v>
       </c>
       <c r="C2" t="str">
         <v>Mumbai</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ShubhamTest</v>
-      </c>
-      <c r="B3" t="str">
-        <v>060087218145</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Singapore</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SUBJECT: OpenTelemetry implemented MESSAGE: Jaeger integration done -> To run Jaeger , go to cmd and run all in one exe file or run jaeger from docker
</commit_message>
<xml_diff>
--- a/reportData.xlsx
+++ b/reportData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,26 +407,59 @@
         <v>resourceName</v>
       </c>
       <c r="B1" t="str">
-        <v>accountId</v>
+        <v>accountIds</v>
       </c>
       <c r="C1" t="str">
-        <v>region</v>
+        <v>regions</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>shubhamTest</v>
-      </c>
-      <c r="B2">
-        <v>3438</v>
+        <v>testResource</v>
+      </c>
+      <c r="B2" t="str">
+        <v>060087218145</v>
       </c>
       <c r="C2" t="str">
+        <v>Mumbai</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>resourceSingapore</v>
+      </c>
+      <c r="B3" t="str">
+        <v>060087218145</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Singapore</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>ShubhamTest</v>
+      </c>
+      <c r="B4" t="str">
+        <v>060087218145</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Singapore</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>resourceMumbai</v>
+      </c>
+      <c r="B5" t="str">
+        <v>060087218145</v>
+      </c>
+      <c r="C5" t="str">
         <v>Mumbai</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>